<commit_message>
added prefixes to enviroment variables
</commit_message>
<xml_diff>
--- a/codes/stream/Errors.xlsx
+++ b/codes/stream/Errors.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lc432959\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Desktop\repos\ba-raimbault-task-affinity\codes\stream\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,8 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="28">
   <si>
     <t>conf. (0,0,0,0)</t>
   </si>
@@ -102,12 +103,18 @@
   </si>
   <si>
     <t>decode weight</t>
+  </si>
+  <si>
+    <t>For one Thread</t>
+  </si>
+  <si>
+    <t>For all Threads</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -155,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -172,6 +179,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -456,32 +469,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="13.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="3.5703125" style="4" customWidth="1"/>
-    <col min="7" max="9" width="11.42578125" style="5"/>
-    <col min="10" max="10" width="13.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="13.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="3.5546875" style="4" customWidth="1"/>
+    <col min="7" max="9" width="11.44140625" style="5"/>
+    <col min="10" max="10" width="13.21875" style="5" customWidth="1"/>
     <col min="11" max="11" width="15" style="5" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" style="5" customWidth="1"/>
-    <col min="13" max="14" width="17.85546875" style="5" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" style="5"/>
-    <col min="16" max="16" width="1.42578125" style="6" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="15.5546875" style="5" customWidth="1"/>
+    <col min="13" max="14" width="17.77734375" style="5" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" style="5"/>
+    <col min="16" max="16" width="1.44140625" style="6" customWidth="1"/>
+    <col min="17" max="17" width="13.21875" style="5" customWidth="1"/>
     <col min="18" max="18" width="13" style="5" customWidth="1"/>
     <col min="19" max="19" width="12" style="5" customWidth="1"/>
-    <col min="20" max="20" width="13.5703125" style="5" customWidth="1"/>
-    <col min="21" max="21" width="16.28515625" style="5" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" style="1"/>
+    <col min="20" max="20" width="13.5546875" style="5" customWidth="1"/>
+    <col min="21" max="21" width="16.21875" style="5" customWidth="1"/>
+    <col min="22" max="22" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="L1" s="5" t="s">
         <v>24</v>
       </c>
@@ -507,7 +520,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="7" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" s="7" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -538,7 +551,7 @@
       <c r="U2" s="6"/>
       <c r="V2" s="4"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -565,7 +578,7 @@
         <v>16</v>
       </c>
       <c r="L3" s="5">
-        <f t="shared" ref="L3:L4" si="0">_xlfn.NUMBERVALUE(U3)/100</f>
+        <f>_xlfn.NUMBERVALUE(U3)/100</f>
         <v>0</v>
       </c>
       <c r="M3" s="5" t="str">
@@ -573,7 +586,7 @@
         <v>00</v>
       </c>
       <c r="N3" s="5" t="str">
-        <f t="shared" ref="N3:N29" si="1">L3&amp;" "&amp;_xlfn.NUMBERVALUE(M3)</f>
+        <f t="shared" ref="N3:N29" si="0">L3&amp;" "&amp;_xlfn.NUMBERVALUE(M3)</f>
         <v>0 0</v>
       </c>
       <c r="O3" s="5">
@@ -586,11 +599,11 @@
         <v>4</v>
       </c>
       <c r="S3" s="5" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(Q3,$G$3:$G$12,0))</f>
+        <f t="shared" ref="S3:S30" si="1">INDEX($H$3:$H$12,MATCH(Q3,$G$3:$G$12,0))</f>
         <v>00</v>
       </c>
       <c r="T3" s="5" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(R3,$G$3:$G$12,0))</f>
+        <f t="shared" ref="T3:T30" si="2">INDEX($H$3:$H$12,MATCH(R3,$G$3:$G$12,0))</f>
         <v>00</v>
       </c>
       <c r="U3" s="5" t="str">
@@ -598,7 +611,7 @@
         <v>0000</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -625,15 +638,15 @@
         <v>16</v>
       </c>
       <c r="L4" s="5">
-        <f t="shared" si="0"/>
+        <f>_xlfn.NUMBERVALUE(U4)/100</f>
         <v>0</v>
       </c>
       <c r="M4" s="5" t="str">
-        <f t="shared" ref="M4:M30" si="2">RIGHT(U4,2)</f>
+        <f t="shared" ref="M4:M30" si="3">RIGHT(U4,2)</f>
         <v>00</v>
       </c>
       <c r="N4" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0 0</v>
       </c>
       <c r="O4" s="5">
@@ -646,19 +659,19 @@
         <v>4</v>
       </c>
       <c r="S4" s="5" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(Q4,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>00</v>
       </c>
       <c r="T4" s="5" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(R4,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>00</v>
       </c>
       <c r="U4" s="5" t="str">
-        <f t="shared" ref="U4:U30" si="3">S4&amp;""&amp;T4</f>
+        <f t="shared" ref="U4:U30" si="4">S4&amp;""&amp;T4</f>
         <v>0000</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -689,11 +702,11 @@
         <v>5</v>
       </c>
       <c r="M5" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>01</v>
       </c>
       <c r="N5" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5 1</v>
       </c>
       <c r="O5" s="5">
@@ -706,19 +719,19 @@
         <v>11</v>
       </c>
       <c r="S5" s="5">
-        <f>INDEX($H$3:$H$12,MATCH(Q5,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="T5" s="5" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(R5,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>01</v>
       </c>
       <c r="U5" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>501</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -745,15 +758,15 @@
         <v>16</v>
       </c>
       <c r="L6" s="5">
-        <f t="shared" ref="L6:L30" si="4">ROUND(_xlfn.NUMBERVALUE(U6)/100,0)</f>
+        <f t="shared" ref="L6:L30" si="5">ROUND(_xlfn.NUMBERVALUE(U6)/100,0)</f>
         <v>5</v>
       </c>
       <c r="M6" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>01</v>
       </c>
       <c r="N6" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5 1</v>
       </c>
       <c r="O6" s="5">
@@ -766,19 +779,19 @@
         <v>11</v>
       </c>
       <c r="S6" s="5">
-        <f>INDEX($H$3:$H$12,MATCH(Q6,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="T6" s="5" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(R6,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>01</v>
       </c>
       <c r="U6" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>501</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -803,15 +816,15 @@
         <v>16</v>
       </c>
       <c r="L7" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="M7" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>01</v>
       </c>
       <c r="N7" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4 1</v>
       </c>
       <c r="O7" s="5">
@@ -824,19 +837,19 @@
         <v>11</v>
       </c>
       <c r="S7" s="5">
-        <f>INDEX($H$3:$H$12,MATCH(Q7,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="T7" s="5" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(R7,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>01</v>
       </c>
       <c r="U7" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>401</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -865,15 +878,15 @@
         <v>16</v>
       </c>
       <c r="L8" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M8" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="N8" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0 15</v>
       </c>
       <c r="O8" s="8">
@@ -886,19 +899,19 @@
         <v>5</v>
       </c>
       <c r="S8" s="8">
-        <f>INDEX($H$3:$H$12,MATCH(Q8,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="T8" s="8">
-        <f>INDEX($H$3:$H$12,MATCH(R8,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="U8" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -925,15 +938,15 @@
         <v>16</v>
       </c>
       <c r="L9" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M9" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>01</v>
       </c>
       <c r="N9" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1 1</v>
       </c>
       <c r="O9" s="5">
@@ -946,19 +959,19 @@
         <v>11</v>
       </c>
       <c r="S9" s="5">
-        <f>INDEX($H$3:$H$12,MATCH(Q9,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="T9" s="5" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(R9,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>01</v>
       </c>
       <c r="U9" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -986,15 +999,15 @@
         <v>16</v>
       </c>
       <c r="L10" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M10" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>02</v>
       </c>
       <c r="N10" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1 2</v>
       </c>
       <c r="O10" s="5">
@@ -1007,19 +1020,19 @@
         <v>12</v>
       </c>
       <c r="S10" s="5">
-        <f>INDEX($H$3:$H$12,MATCH(Q10,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="T10" s="5" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(R10,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>02</v>
       </c>
       <c r="U10" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1045,15 +1058,15 @@
         <v>16</v>
       </c>
       <c r="L11" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M11" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>03</v>
       </c>
       <c r="N11" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1 3</v>
       </c>
       <c r="O11" s="5">
@@ -1066,19 +1079,19 @@
         <v>13</v>
       </c>
       <c r="S11" s="5">
-        <f>INDEX($H$3:$H$12,MATCH(Q11,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="T11" s="5" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(R11,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>03</v>
       </c>
       <c r="U11" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1108,15 +1121,15 @@
         <v>16</v>
       </c>
       <c r="L12" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M12" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>03</v>
       </c>
       <c r="N12" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1 3</v>
       </c>
       <c r="O12" s="5">
@@ -1129,19 +1142,19 @@
         <v>13</v>
       </c>
       <c r="S12" s="5">
-        <f>INDEX($H$3:$H$12,MATCH(Q12,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="T12" s="5" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(R12,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>03</v>
       </c>
       <c r="U12" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1160,15 +1173,15 @@
         <v>16</v>
       </c>
       <c r="L13" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M13" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>01</v>
       </c>
       <c r="N13" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1 1</v>
       </c>
       <c r="O13" s="5">
@@ -1181,19 +1194,19 @@
         <v>11</v>
       </c>
       <c r="S13" s="5">
-        <f>INDEX($H$3:$H$12,MATCH(Q13,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="T13" s="5" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(R13,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>01</v>
       </c>
       <c r="U13" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1214,15 +1227,15 @@
         <v>16</v>
       </c>
       <c r="L14" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M14" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>01</v>
       </c>
       <c r="N14" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1 1</v>
       </c>
       <c r="O14" s="5">
@@ -1235,19 +1248,19 @@
         <v>11</v>
       </c>
       <c r="S14" s="5">
-        <f>INDEX($H$3:$H$12,MATCH(Q14,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="T14" s="5" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(R14,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>01</v>
       </c>
       <c r="U14" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1266,15 +1279,15 @@
         <v>16</v>
       </c>
       <c r="L15" s="9" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
       <c r="M15" s="9" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="N15" s="9" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="O15" s="9">
@@ -1287,19 +1300,19 @@
         <v>14</v>
       </c>
       <c r="S15" s="9">
-        <f>INDEX($H$3:$H$12,MATCH(Q15,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="T15" s="9" t="e">
-        <f>INDEX($H$3:$H$12,MATCH(R15,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="U15" s="9" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1318,15 +1331,15 @@
         <v>16</v>
       </c>
       <c r="L16" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="M16" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>03</v>
       </c>
       <c r="N16" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3 3</v>
       </c>
       <c r="O16" s="5">
@@ -1339,19 +1352,19 @@
         <v>13</v>
       </c>
       <c r="S16" s="5">
-        <f>INDEX($H$3:$H$12,MATCH(Q16,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="T16" s="5" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(R16,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>03</v>
       </c>
       <c r="U16" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>303</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1372,15 +1385,15 @@
         <v>16</v>
       </c>
       <c r="L17" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M17" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="N17" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0 25</v>
       </c>
       <c r="O17" s="8">
@@ -1393,19 +1406,19 @@
         <v>5</v>
       </c>
       <c r="S17" s="8">
-        <f>INDEX($H$3:$H$12,MATCH(Q17,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="T17" s="8">
-        <f>INDEX($H$3:$H$12,MATCH(R17,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="U17" s="8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1424,15 +1437,15 @@
         <v>16</v>
       </c>
       <c r="L18" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="M18" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>01</v>
       </c>
       <c r="N18" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2 1</v>
       </c>
       <c r="O18" s="5">
@@ -1445,19 +1458,19 @@
         <v>11</v>
       </c>
       <c r="S18" s="5">
-        <f>INDEX($H$3:$H$12,MATCH(Q18,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="T18" s="5" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(R18,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>01</v>
       </c>
       <c r="U18" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>201</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1474,15 +1487,15 @@
         <v>16</v>
       </c>
       <c r="L19" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="M19" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>01</v>
       </c>
       <c r="N19" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2 1</v>
       </c>
       <c r="O19" s="5">
@@ -1495,19 +1508,19 @@
         <v>11</v>
       </c>
       <c r="S19" s="5">
-        <f>INDEX($H$3:$H$12,MATCH(Q19,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="T19" s="5" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(R19,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>01</v>
       </c>
       <c r="U19" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>201</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1530,15 +1543,15 @@
         <v>16</v>
       </c>
       <c r="L20" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="M20" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>02</v>
       </c>
       <c r="N20" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2 2</v>
       </c>
       <c r="O20" s="5">
@@ -1551,19 +1564,19 @@
         <v>12</v>
       </c>
       <c r="S20" s="5">
-        <f>INDEX($H$3:$H$12,MATCH(Q20,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="T20" s="5" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(R20,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>02</v>
       </c>
       <c r="U20" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1582,15 +1595,15 @@
         <v>16</v>
       </c>
       <c r="L21" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="M21" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>03</v>
       </c>
       <c r="N21" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2 3</v>
       </c>
       <c r="O21" s="5">
@@ -1603,19 +1616,19 @@
         <v>13</v>
       </c>
       <c r="S21" s="5">
-        <f>INDEX($H$3:$H$12,MATCH(Q21,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="T21" s="5" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(R21,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>03</v>
       </c>
       <c r="U21" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>203</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1634,15 +1647,15 @@
         <v>16</v>
       </c>
       <c r="L22" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M22" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="N22" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1 25</v>
       </c>
       <c r="O22" s="9">
@@ -1655,19 +1668,19 @@
         <v>5</v>
       </c>
       <c r="S22" s="9">
-        <f>INDEX($H$3:$H$12,MATCH(Q22,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="T22" s="9">
-        <f>INDEX($H$3:$H$12,MATCH(R22,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="U22" s="9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1684,15 +1697,15 @@
         <v>16</v>
       </c>
       <c r="L23" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="M23" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>01</v>
       </c>
       <c r="N23" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12 1</v>
       </c>
       <c r="O23" s="9">
@@ -1705,19 +1718,19 @@
         <v>11</v>
       </c>
       <c r="S23" s="9">
-        <f>INDEX($H$3:$H$12,MATCH(Q23,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="T23" s="9" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(R23,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>01</v>
       </c>
       <c r="U23" s="9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1201</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1736,15 +1749,15 @@
         <v>16</v>
       </c>
       <c r="L24" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="M24" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>02</v>
       </c>
       <c r="N24" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12 2</v>
       </c>
       <c r="O24" s="9">
@@ -1757,19 +1770,19 @@
         <v>12</v>
       </c>
       <c r="S24" s="9">
-        <f>INDEX($H$3:$H$12,MATCH(Q24,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="T24" s="9" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(R24,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>02</v>
       </c>
       <c r="U24" s="9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1202</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1788,15 +1801,15 @@
         <v>16</v>
       </c>
       <c r="L25" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="M25" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>03</v>
       </c>
       <c r="N25" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12 3</v>
       </c>
       <c r="O25" s="9">
@@ -1809,19 +1822,19 @@
         <v>13</v>
       </c>
       <c r="S25" s="9">
-        <f>INDEX($H$3:$H$12,MATCH(Q25,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="T25" s="9" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(R25,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>03</v>
       </c>
       <c r="U25" s="9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1203</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1842,15 +1855,15 @@
         <v>16</v>
       </c>
       <c r="L26" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M26" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="N26" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0 35</v>
       </c>
       <c r="O26" s="8">
@@ -1863,19 +1876,19 @@
         <v>5</v>
       </c>
       <c r="S26" s="8">
-        <f>INDEX($H$3:$H$12,MATCH(Q26,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="T26" s="8">
-        <f>INDEX($H$3:$H$12,MATCH(R26,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="U26" s="8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1896,15 +1909,15 @@
         <v>16</v>
       </c>
       <c r="L27" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="M27" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>01</v>
       </c>
       <c r="N27" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3 1</v>
       </c>
       <c r="O27" s="5">
@@ -1917,19 +1930,19 @@
         <v>11</v>
       </c>
       <c r="S27" s="5">
-        <f>INDEX($H$3:$H$12,MATCH(Q27,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="T27" s="5" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(R27,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>01</v>
       </c>
       <c r="U27" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>301</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1950,15 +1963,15 @@
         <v>16</v>
       </c>
       <c r="L28" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="M28" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>01</v>
       </c>
       <c r="N28" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3 1</v>
       </c>
       <c r="O28" s="5">
@@ -1971,19 +1984,19 @@
         <v>11</v>
       </c>
       <c r="S28" s="5">
-        <f>INDEX($H$3:$H$12,MATCH(Q28,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="T28" s="5" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(R28,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>01</v>
       </c>
       <c r="U28" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>301</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2000,15 +2013,15 @@
         <v>16</v>
       </c>
       <c r="L29" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="M29" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>02</v>
       </c>
       <c r="N29" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3 2</v>
       </c>
       <c r="O29" s="5">
@@ -2021,19 +2034,19 @@
         <v>12</v>
       </c>
       <c r="S29" s="5">
-        <f>INDEX($H$3:$H$12,MATCH(Q29,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="T29" s="5" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(R29,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>02</v>
       </c>
       <c r="U29" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>302</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2056,11 +2069,11 @@
         <v>16</v>
       </c>
       <c r="L30" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="M30" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>03</v>
       </c>
       <c r="N30" s="5" t="str">
@@ -2077,19 +2090,19 @@
         <v>13</v>
       </c>
       <c r="S30" s="5">
-        <f>INDEX($H$3:$H$12,MATCH(Q30,$G$3:$G$12,0))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="T30" s="5" t="str">
-        <f>INDEX($H$3:$H$12,MATCH(R30,$G$3:$G$12,0))</f>
+        <f t="shared" si="2"/>
         <v>03</v>
       </c>
       <c r="U30" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>303</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2102,7 +2115,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2116,8 +2129,15 @@
         <v>1.27</v>
       </c>
       <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="T32" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="U32" s="10">
+        <f>20/(5*2*5*4)</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2129,6 +2149,13 @@
         <v>2.16</v>
       </c>
       <c r="E33" s="2"/>
+      <c r="T33" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="U33" s="11">
+        <f>U32/30</f>
+        <v>3.3333333333333335E-3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>